<commit_message>
Sigue la preparación de los posters
</commit_message>
<xml_diff>
--- a/complete_data.xlsx
+++ b/complete_data.xlsx
@@ -793,7 +793,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAAEAAAABCAYAAAAfFcSJAAAADUlEQVR42mP8+fPbfwAJxAPp1plWegAAAABJRU5ErkJggg==</t>
+          <t>https://www.soriana.com/dw/image/v2/BGBD_PRD/on/demandware.static/-/Sites-soriana-grocery-master-catalog/default/dwaaae9371/images/product/8806091641540_A.jpg?sw=106&amp;sh=106&amp;sm=fit</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -3016,11 +3016,11 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Hisense Smart TV LED A6H 55", 4K Ultra HD, Negro</t>
+          <t>Samsung Smart TV LED CU7000 50", 4K Ultra HD, Negro</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>7419</v>
+        <v>7469</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -3029,7 +3029,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>https://www.cyberpuerta.mx/img/product/S/CP-HISENSE-55A6H-1612b6.jpg</t>
+          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-UN50CU7000FXZX-eb870a.jpg</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -3039,18 +3039,18 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>: 139,7 cm (55")</t>
+          <t>: 127 cm (50")</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Samsung Smart TV LED CU7000 50", 4K Ultra HD, Negro</t>
+          <t>Samsung Smart TV LED CU7000 85", 4K Ultra HD, Negro</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>7469</v>
+        <v>24349</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -3059,7 +3059,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-UN50CU7000FXZX-eb870a.jpg</t>
+          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-UN85CU7000FXZX-eb870a.jpg</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -3069,18 +3069,18 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>: 127 cm (50")</t>
+          <t>: 216 cm (85")</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Samsung Smart TV LED CU7000 85", 4K Ultra HD, Negro</t>
+          <t>﻿Samsung Smart TV LED CU7000 43", 4K Ultra HD, Negro</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>24349</v>
+        <v>6249</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -3089,7 +3089,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-UN85CU7000FXZX-eb870a.jpg</t>
+          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-UN43CU7000FXZX-eb870a.jpg</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -3099,18 +3099,18 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>: 216 cm (85")</t>
+          <t>: 109,2 cm (43")</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>﻿Samsung Smart TV LED CU7000 43", 4K Ultra HD, Negro</t>
+          <t>Insignia Smart TV LED F30 58", 4K Ultra HD, Negro</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>6249</v>
+        <v>6029</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
@@ -3119,7 +3119,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-UN43CU7000FXZX-eb870a.jpg</t>
+          <t>https://www.cyberpuerta.mx/img/product/S/CP-INSIGNIA-NS-58F301NA22-3e1d09.jpg</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -3129,18 +3129,18 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>: 109,2 cm (43")</t>
+          <t>: 147.3 cm (58")</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Insignia Smart TV LED F30 58", 4K Ultra HD, Negro</t>
+          <t>Samsung Smart TV LED CU7010 43", 4K Ultra HD, Negro</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>6029</v>
+        <v>7449</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -3149,7 +3149,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>https://www.cyberpuerta.mx/img/product/S/CP-INSIGNIA-NS-58F301NA22-3e1d09.jpg</t>
+          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-UN50CU7010FXZX-eb6839.jpg</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -3159,18 +3159,18 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>: 147.3 cm (58")</t>
+          <t>: 127 cm (50")</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Samsung Smart TV LED CU7010 43", 4K Ultra HD, Negro</t>
+          <t>Samsung Smart TV LED CU7000 70", 4K Ultra HD, Negro</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>7449</v>
+        <v>13939</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
@@ -3179,7 +3179,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-UN50CU7010FXZX-eb6839.jpg</t>
+          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-UN70CU7000FXZX-eb870a.jpg</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -3189,18 +3189,18 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>: 127 cm (50")</t>
+          <t>: 177.8 cm (70")</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Samsung Smart TV LED CU7000 70", 4K Ultra HD, Negro</t>
+          <t>LG Smart TV LED UHD AI ThinQ UQ80 55", 4K Ultra HD, Negro</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>13939</v>
+        <v>7879</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
@@ -3209,7 +3209,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-UN70CU7000FXZX-eb870a.jpg</t>
+          <t>https://www.cyberpuerta.mx/img/product/S/CP-LG-55UQ8000PSB-490ab8.jpg</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -3219,18 +3219,18 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>: 177.8 cm (70")</t>
+          <t>: 139,7 cm (55")</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>LG Smart TV LED UHD AI ThinQ UQ80 55", 4K Ultra HD, Negro</t>
+          <t>Vizio Smart TV LED V-Series 75", 4K Ultra HD, Negro</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>7879</v>
+        <v>12749</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
@@ -3239,7 +3239,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>https://www.cyberpuerta.mx/img/product/S/CP-LG-55UQ8000PSB-490ab8.jpg</t>
+          <t>https://www.cyberpuerta.mx/img/product/S/CP-VIZIO-V755-J04-b54181.jpg</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -3249,18 +3249,18 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>: 139,7 cm (55")</t>
+          <t>: 190,5 cm (75")</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Vizio Smart TV LED V-Series 75", 4K Ultra HD, Negro</t>
+          <t>LG Smart TV LED AI ThinQ 60", 4K Ultra HD, Negro</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>12749</v>
+        <v>9459</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
@@ -3269,7 +3269,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>https://www.cyberpuerta.mx/img/product/S/CP-VIZIO-V755-J04-b54181.jpg</t>
+          <t>https://www.cyberpuerta.mx/img/product/S/CP-LG-60UQ8000PSB-f2b139.jpg</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -3279,18 +3279,18 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>: 190,5 cm (75")</t>
+          <t>: 152.4 cm (60")</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>LG Smart TV LED AI ThinQ 60", 4K Ultra HD, Negro</t>
+          <t>﻿Samsung Smart TV Neo QLED QN90C 55", 4K Ultra HD, Plata</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>9459</v>
+        <v>22979</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
@@ -3299,7 +3299,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>https://www.cyberpuerta.mx/img/product/S/CP-LG-60UQ8000PSB-f2b139.jpg</t>
+          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-QN55QN90CAFXZX-096ced.jpg</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -3309,18 +3309,18 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>: 152.4 cm (60")</t>
+          <t>: 139,7 cm (55")</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>﻿Samsung Smart TV Neo QLED QN90C 55", 4K Ultra HD, Plata</t>
+          <t>Hisense Smart TV LED A60GV 43", 4K Ultra HD, Negro</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>22979</v>
+        <v>5919</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
@@ -3329,7 +3329,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-QN55QN90CAFXZX-096ced.jpg</t>
+          <t>https://www.cyberpuerta.mx/img/product/S/CP-HISENSE-43A60GV-af5f3e.png</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -3339,18 +3339,18 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>: 139,7 cm (55")</t>
+          <t>: 109,2 cm (43")</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Hisense Smart TV LED A60GV 43", 4K Ultra HD, Negro</t>
+          <t>Samsung Smart TV LED AU8000 55", 4K Ultra HD, Negro</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>5919</v>
+        <v>11429</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
@@ -3359,7 +3359,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>https://www.cyberpuerta.mx/img/product/S/CP-HISENSE-43A60GV-af5f3e.png</t>
+          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-HG55AU800NFXZA-5bd414.jpg</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -3369,18 +3369,18 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>: 109,2 cm (43")</t>
+          <t>: 139,7 cm (55")</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Samsung Smart TV LED AU8000 55", 4K Ultra HD, Negro</t>
+          <t>Samsung Smart TV LED QN90A Neo QLED 75", 4K Ultra HD, Negro</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>11429</v>
+        <v>26349</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
@@ -3389,7 +3389,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-HG55AU800NFXZA-5bd414.jpg</t>
+          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-QN75QN90AAFXZX-acb76d.jpg</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
@@ -3399,18 +3399,18 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>: 139,7 cm (55")</t>
+          <t>: 189.2 cm (74.5")</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Samsung Smart TV LED QN90A Neo QLED 75", 4K Ultra HD, Negro</t>
+          <t>Samsung Smart TV QLED Q70C 65", 4K Ultra HD, Negro</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>26349</v>
+        <v>15869</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
@@ -3419,7 +3419,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-QN75QN90AAFXZX-acb76d.jpg</t>
+          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-QN65Q70CAFXZX-721b23.jpg</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -3429,18 +3429,18 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>: 189.2 cm (74.5")</t>
+          <t>: 165.1 cm (65")</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Samsung Smart TV QLED Q70C 65", 4K Ultra HD, Negro</t>
+          <t>Samsung Smart TV LED AU8000 Crystal 70", 4K Ultra HD, Negro</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>15869</v>
+        <v>15719</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
@@ -3449,7 +3449,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-QN65Q70CAFXZX-721b23.jpg</t>
+          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-UN70AU8000FXZX-5cdea9.jpg</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -3459,18 +3459,18 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>: 165.1 cm (65")</t>
+          <t>: 177.8 cm (70")</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Samsung Smart TV LED AU8000 Crystal 70", 4K Ultra HD, Negro</t>
+          <t>Xiaomi Smart TV LED A Pro 55 55", 4K Ultra HD, Negro</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>15719</v>
+        <v>7689</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>https://www.cyberpuerta.mx/img/product/S/CP-SAMSUNG-UN70AU8000FXZX-5cdea9.jpg</t>
+          <t>https://www.cyberpuerta.mx/img/product/S/CP-XIAOMI-L55M8-A2LA-0b4b8c.jpg</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -3489,7 +3489,7 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>: 177.8 cm (70")</t>
+          <t>: 139,7 cm (55")</t>
         </is>
       </c>
     </row>

</xml_diff>